<commit_message>
exit blocks added to excel
</commit_message>
<xml_diff>
--- a/src/Track/TrackModel/redline_layout.xlsx
+++ b/src/Track/TrackModel/redline_layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeone\Documents\ECE1140ChooChoo\src\Track\TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632E0B96-8DB2-473A-B5BB-EF523CBF9837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716059FC-10D8-46C0-BEA2-1FA94C7552D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
+    <workbookView xWindow="11916" yWindow="0" windowWidth="11220" windowHeight="12336" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521756E0-942E-44A0-8B9B-C1C5C2AAFFBA}">
   <dimension ref="A1:S153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="74" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="Q48" sqref="Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1955,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="Q25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R25">
         <f t="shared" si="1"/>
@@ -2360,7 +2360,7 @@
         <v>2</v>
       </c>
       <c r="Q33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R33">
         <f t="shared" si="1"/>
@@ -2965,7 +2965,7 @@
         <v>2</v>
       </c>
       <c r="Q45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R45">
         <f t="shared" si="1"/>
@@ -3116,7 +3116,7 @@
         <v>3</v>
       </c>
       <c r="Q48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R48">
         <f t="shared" si="1"/>
@@ -4116,7 +4116,7 @@
         <v>3</v>
       </c>
       <c r="Q68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R68">
         <f t="shared" si="3"/>
@@ -4313,7 +4313,7 @@
         <v>2</v>
       </c>
       <c r="Q72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R72">
         <f t="shared" si="3"/>
@@ -4366,7 +4366,7 @@
         <v>2</v>
       </c>
       <c r="Q73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R73">
         <f t="shared" si="3"/>
@@ -4563,7 +4563,7 @@
         <v>1</v>
       </c>
       <c r="Q77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R77">
         <f t="shared" si="3"/>
@@ -4614,7 +4614,7 @@
         <v>1</v>
       </c>
       <c r="Q78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R78">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
redline plc program work
</commit_message>
<xml_diff>
--- a/src/Track/TrackModel/redline_layout.xlsx
+++ b/src/Track/TrackModel/redline_layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeone\Documents\ECE1140ChooChoo\src\Track\TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716059FC-10D8-46C0-BEA2-1FA94C7552D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB0EB39-2353-4125-AC34-8BD42E96A412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11916" yWindow="0" windowWidth="11220" windowHeight="12336" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="11304" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -195,9 +195,6 @@
     <t>Station Square</t>
   </si>
   <si>
-    <t>16-15,16-1</t>
-  </si>
-  <si>
     <t>27-28,27-76</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>R72</t>
+  </si>
+  <si>
+    <t>16-1,16-15</t>
   </si>
 </sst>
 </file>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521756E0-942E-44A0-8B9B-C1C5C2AAFFBA}">
   <dimension ref="A1:S153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="Q48" sqref="Q48"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="74" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +784,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K2" s="4">
         <v>1</v>
@@ -797,7 +797,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O2" s="4">
         <v>0</v>
@@ -1184,7 +1184,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K10" s="4">
         <v>0</v>
@@ -1236,7 +1236,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K11" s="4">
         <v>1</v>
@@ -1249,7 +1249,7 @@
         <v>1</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O11" s="4">
         <v>0</v>
@@ -1484,7 +1484,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="J16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K16" s="4">
         <v>1</v>
@@ -1538,7 +1538,7 @@
         <v>2</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="K17" s="4">
         <v>0</v>
@@ -2088,7 +2088,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K28" s="4">
         <v>0</v>
@@ -2140,7 +2140,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K29" s="4">
         <v>1</v>
@@ -2153,7 +2153,7 @@
         <v>1</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O29" s="4">
         <v>1</v>
@@ -2341,7 +2341,7 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K33" s="4">
         <v>1</v>
@@ -2391,7 +2391,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K34" s="4">
         <v>0</v>
@@ -2642,7 +2642,7 @@
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
       <c r="I39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K39" s="4">
         <v>0</v>
@@ -2694,7 +2694,7 @@
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K40" s="4">
         <v>1</v>
@@ -2707,7 +2707,7 @@
         <v>1</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O40" s="4">
         <v>1</v>
@@ -2895,7 +2895,7 @@
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K44" s="4">
         <v>1</v>
@@ -2945,7 +2945,7 @@
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K45" s="4">
         <v>0</v>
@@ -3347,7 +3347,7 @@
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K53" s="4">
         <v>0</v>
@@ -3399,7 +3399,7 @@
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="J54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K54" s="4">
         <v>1</v>
@@ -3412,7 +3412,7 @@
         <v>1</v>
       </c>
       <c r="N54" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O54" s="4">
         <v>0</v>
@@ -4043,7 +4043,7 @@
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="J67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K67" s="4">
         <v>1</v>
@@ -4094,7 +4094,7 @@
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
       <c r="J68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K68" s="4">
         <v>1</v>
@@ -4107,7 +4107,7 @@
         <v>1</v>
       </c>
       <c r="N68" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O68" s="4">
         <v>1</v>
@@ -4294,7 +4294,7 @@
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="J72" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K72" s="4">
         <v>1</v>
@@ -4345,7 +4345,7 @@
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="J73" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K73" s="4">
         <v>1</v>
@@ -4357,7 +4357,7 @@
         <v>1</v>
       </c>
       <c r="N73" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O73" s="4">
         <v>1</v>
@@ -4544,7 +4544,7 @@
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
       <c r="J77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K77" s="4">
         <v>1</v>
@@ -4595,7 +4595,7 @@
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
       <c r="J78" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K78" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
fixed clamping for greenline entrance and more work on the red line plc
</commit_message>
<xml_diff>
--- a/src/Track/TrackModel/redline_layout.xlsx
+++ b/src/Track/TrackModel/redline_layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeone\Documents\ECE1140ChooChoo\src\Track\TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1104945-A7BB-4C2F-98D9-E56D487D82D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C31EBB9-EFE3-4680-AFB4-9E9526893B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
+    <workbookView xWindow="1464" yWindow="936" windowWidth="17280" windowHeight="11304" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521756E0-942E-44A0-8B9B-C1C5C2AAFFBA}">
   <dimension ref="A1:T153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="V69" sqref="V69"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>